<commit_message>
1131_Maximum of Absolute Value Expression
</commit_message>
<xml_diff>
--- a/DSAP/Documents/DSAQ.xlsx
+++ b/DSAP/Documents/DSAQ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devsa\source\repos\Interview\DSAP\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA410920-23D0-460A-B0AA-8F5C92F77761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A653488-EB9E-4863-96D9-32C7ED09D4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>SNO</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>QNO</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Maximum of Absolute Value Expression</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-of-absolute-value-expression/</t>
   </si>
 </sst>
 </file>
@@ -423,7 +432,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,8 +441,8 @@
     <col min="2" max="2" width="10.77734375" customWidth="1"/>
     <col min="3" max="3" width="11.88671875" customWidth="1"/>
     <col min="4" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="49.21875" customWidth="1"/>
+    <col min="6" max="6" width="38.77734375" customWidth="1"/>
+    <col min="7" max="7" width="65.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -489,14 +498,30 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1131</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>

</xml_diff>